<commit_message>
Add new input system override path(key)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/Stage1/ep00.xlsx
+++ b/Assets/Editor/JsonUtility/Stage1/ep00.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Json\Stage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109706A1-7E2F-4E2A-B798-8A8B5A8B6A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC94D374-6744-49FA-8C4D-846BA4014BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,6 +73,14 @@
   </si>
   <si>
     <t>ttt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕안녕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워반가워</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,7 +559,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -589,16 +597,16 @@
       <c r="A5">
         <v>33</v>
       </c>
-      <c r="B5">
-        <v>122</v>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>22</v>
       </c>
-      <c r="B6">
-        <v>12323</v>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>